<commit_message>
Update GPS-RCB-F9T_rev.1.0_BOM 2025-04-23 18-37.xlsx
</commit_message>
<xml_diff>
--- a/Time-Card ТЕНШ.467883.01/ГНСС МОДУЛИ/UBlox/ТЕНШ.468157.03 RCB-F9T/Altium/ECAD/V1/Project Outputs for GPS-RCB-F9T/GPS-RCB-F9T_rev.1.0_BOM 2025-04-23 18-37.xlsx
+++ b/Time-Card ТЕНШ.467883.01/ГНСС МОДУЛИ/UBlox/ТЕНШ.468157.03 RCB-F9T/Altium/ECAD/V1/Project Outputs for GPS-RCB-F9T/GPS-RCB-F9T_rev.1.0_BOM 2025-04-23 18-37.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Altium\SM_Project\QUANTUM\Time-Card ТЕНШ.467883.001\ГНСС МОДУЛИ\UBlox\ТЕНШ.468157.03 RCB-F9T\Altium\ECAD\V1\Project Outputs for GPS-RCB-F9T\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIWA\Documents\GitHub\QUANTUM\Time-Card ТЕНШ.467883.01\ГНСС МОДУЛИ\UBlox\ТЕНШ.468157.03 RCB-F9T\Altium\ECAD\V1\Project Outputs for GPS-RCB-F9T\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67816B5D-2944-4026-96EC-233866D9CAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA579A3C-3102-4617-A7F6-679429897BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1146" yWindow="1104" windowWidth="17280" windowHeight="9990" xr2:uid="{B3B15BF4-F252-49B9-9BBA-89E86608400D}"/>
+    <workbookView xWindow="0" yWindow="1860" windowWidth="23040" windowHeight="10380" xr2:uid="{B3B15BF4-F252-49B9-9BBA-89E86608400D}"/>
   </bookViews>
   <sheets>
     <sheet name="GPS-RCB-F9T_rev.1.0_BOM 2025-04" sheetId="1" r:id="rId1"/>
@@ -138,15 +138,9 @@
     <t>J2</t>
   </si>
   <si>
-    <t>SMB_131-3711-301</t>
-  </si>
-  <si>
     <t>Rf Coaxial Board Mount Connector</t>
   </si>
   <si>
-    <t>CONN_131-3711-301</t>
-  </si>
-  <si>
     <t>L1</t>
   </si>
   <si>
@@ -289,6 +283,12 @@
   </si>
   <si>
     <t>CMP-0055-01065-3</t>
+  </si>
+  <si>
+    <t>142-0711-301</t>
+  </si>
+  <si>
+    <t>CONN_142-0711-301</t>
   </si>
 </sst>
 </file>
@@ -668,18 +668,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D24F749-24BE-4BEF-89A7-0B9A278D1E8B}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="18.26171875" customWidth="1"/>
-    <col min="5" max="5" width="27.83984375" customWidth="1"/>
-    <col min="6" max="6" width="9.26171875" customWidth="1"/>
-    <col min="7" max="7" width="27.1015625" customWidth="1"/>
-    <col min="8" max="8" width="15.3125" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" customWidth="1"/>
+    <col min="5" max="5" width="27.88671875" customWidth="1"/>
+    <col min="6" max="6" width="9.21875" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -705,7 +710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -727,7 +732,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -749,7 +754,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -771,7 +776,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -795,7 +800,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -817,21 +822,21 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="F7" s="1">
         <v>1</v>
@@ -839,21 +844,21 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="F8" s="1">
         <v>1</v>
@@ -861,21 +866,21 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="F9" s="1">
         <v>3</v>
@@ -883,21 +888,21 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
@@ -905,21 +910,21 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="F11" s="1">
         <v>6</v>
@@ -927,21 +932,21 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="F12" s="1">
         <v>5</v>
@@ -949,21 +954,21 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
@@ -971,21 +976,21 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>
@@ -993,21 +998,21 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E15" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1">
         <v>1</v>
@@ -1015,21 +1020,21 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="F16" s="1">
         <v>2</v>
@@ -1037,21 +1042,21 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="F17" s="1">
         <v>1</v>

</xml_diff>